<commit_message>
added friends in correct position
</commit_message>
<xml_diff>
--- a/map/mundo.xlsx
+++ b/map/mundo.xlsx
@@ -396,8 +396,8 @@
   </sheetPr>
   <dimension ref="A1:AP42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V33" activeCellId="0" sqref="V33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.00390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>